<commit_message>
DNC; added few more functions
</commit_message>
<xml_diff>
--- a/rebuilding_ebo_vbo.xlsx
+++ b/rebuilding_ebo_vbo.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24030"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="15315" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="26660"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="153">
   <si>
     <t>ebo</t>
   </si>
@@ -138,9 +143,6 @@
     <t>t_mesh</t>
   </si>
   <si>
-    <t>usage;</t>
-  </si>
-  <si>
     <t>program;</t>
   </si>
   <si>
@@ -402,6 +404,9 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
       <rPr>
         <b/>
         <sz val="11"/>
@@ -410,6 +415,350 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>sp_build_ebo_normals</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(vao);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sp_build_vbo_normals</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(vao);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sp_build_vbo_normals</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(vao);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sp_rebuild_vbo_from_groups</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(vao);</t>
+    </r>
+  </si>
+  <si>
+    <t>meshes/</t>
+  </si>
+  <si>
+    <t>recenter_positions;</t>
+  </si>
+  <si>
+    <t>if (vao-&gt;recenter_positions)</t>
+  </si>
+  <si>
+    <t>positions_recentering.c</t>
+  </si>
+  <si>
+    <t>processings/</t>
+  </si>
+  <si>
+    <t>normals_calculations_ebo.c</t>
+  </si>
+  <si>
+    <t>normals_calculations_vbo.c</t>
+  </si>
+  <si>
+    <t>groups_calculations.c</t>
+  </si>
+  <si>
+    <t>vbo_rebuilding.c</t>
+  </si>
+  <si>
+    <t>primary_vao.c</t>
+  </si>
+  <si>
+    <t>final_vao_construction.c</t>
+  </si>
+  <si>
+    <t>final_vao_push.c</t>
+  </si>
+  <si>
+    <t>remove</t>
+  </si>
+  <si>
+    <t>uv_calculations.c</t>
+  </si>
+  <si>
+    <t>positions_calculations.c</t>
+  </si>
+  <si>
+    <t>normals_calculation.c</t>
+  </si>
+  <si>
+    <t>mesh_vbo_operations.c</t>
+  </si>
+  <si>
+    <t>mesh_refresh.c</t>
+  </si>
+  <si>
+    <t>update</t>
+  </si>
+  <si>
+    <t>mesh_operations.c</t>
+  </si>
+  <si>
+    <t>mesh_dumb_fill.c</t>
+  </si>
+  <si>
+    <t>mesh_creation.c</t>
+  </si>
+  <si>
+    <t>buffer_generated;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    glGenVertexArrays(1, me-&gt;handles + 0);</t>
+  </si>
+  <si>
+    <t>if (!me-&gt;buff_generated)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    glGenBuffers(1, me-&gt;handles + 1);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    glGenBuffers(1, me-&gt;handles + 2);</t>
+  </si>
+  <si>
+    <t>vali[1];</t>
+  </si>
+  <si>
+    <t>valf[1];</t>
+  </si>
+  <si>
+    <t>(*set_groups)(t_vao_basic *vao);</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>if (vao-&gt;set_groups != NULL)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>vao-&gt;set_groups</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(vao);</t>
+    </r>
+  </si>
+  <si>
+    <t>(*set_tex)(t_vao_basic *vao);</t>
+  </si>
+  <si>
+    <t>if (ntex_req != vao-&gt;vbo.ntex &amp;&amp; vao-&gt;set_tex != NULL)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>vao-&gt;set_tex</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(vao);</t>
+    </r>
+  </si>
+  <si>
+    <t>receiving: (t_vao_basic *vao)</t>
+  </si>
+  <si>
+    <t>split_vbo(vao);</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">if (vao-&gt;fill == NULL || </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>vao-&gt;fill</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(me, vao))</t>
+    </r>
+  </si>
+  <si>
+    <t>textures_calculations_utility.c</t>
+  </si>
+  <si>
+    <t>textures_calculations.c</t>
+  </si>
+  <si>
+    <t>static inline split_vbo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <r>
+      <t>if (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>validate_vbo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(&amp;vao-&gt;vbo, vs)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>push_attributes</t>
     </r>
     <r>
@@ -425,18 +774,26 @@
   </si>
   <si>
     <r>
-      <t>if (</t>
+      <t>t_byte const vbo_width =</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>validate_vbo</t>
+        <color rgb="FF008000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>calc_vbo_width</t>
     </r>
     <r>
       <rPr>
@@ -446,7 +803,57 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(&amp;vao-&gt;vbo, vs)</t>
+      <t>(&amp;vao-&gt;vbo);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sp_recenter_positions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(&amp;vao-&gt;vbo);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ftv_foreach(&amp;vao-&gt;ebo.faces, &amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fill_ebo_final</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, ebo_final);</t>
     </r>
   </si>
   <si>
@@ -457,9 +864,8 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <color rgb="FF008000"/>
+        <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
       <t>fill_vbo_final</t>
@@ -474,411 +880,13 @@
       </rPr>
       <t>, vbo_final, &amp;vao-&gt;vbo);</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t>ftv_foreach(&amp;vao-&gt;ebo.faces, &amp;</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>fill_ebo_final</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, ebo_final);</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">t_byte const vbo_width = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>calc_vbo_width</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(&amp;vao-&gt;vbo);</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>sp_build_ebo_normals</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(vao);</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>sp_build_vbo_normals</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(vao);</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">        </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>sp_build_vbo_normals</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(vao);</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>sp_rebuild_vbo_from_groups</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(vao);</t>
-    </r>
-  </si>
-  <si>
-    <t>meshes/</t>
-  </si>
-  <si>
-    <t>recenter_positions;</t>
-  </si>
-  <si>
-    <t>if (vao-&gt;recenter_positions)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>sp_recenter_positions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(&amp;vao-&gt;vbo);</t>
-    </r>
-  </si>
-  <si>
-    <t>positions_recentering.c</t>
-  </si>
-  <si>
-    <t>processings/</t>
-  </si>
-  <si>
-    <t>normals_calculations_ebo.c</t>
-  </si>
-  <si>
-    <t>normals_calculations_vbo.c</t>
-  </si>
-  <si>
-    <t>groups_calculations.c</t>
-  </si>
-  <si>
-    <t>vbo_rebuilding.c</t>
-  </si>
-  <si>
-    <t>primary_vao.c</t>
-  </si>
-  <si>
-    <t>final_vao_construction.c</t>
-  </si>
-  <si>
-    <t>final_vao_push.c</t>
-  </si>
-  <si>
-    <t>remove</t>
-  </si>
-  <si>
-    <t>uv_calculations.c</t>
-  </si>
-  <si>
-    <t>positions_calculations.c</t>
-  </si>
-  <si>
-    <t>normals_calculation.c</t>
-  </si>
-  <si>
-    <t>mesh_vbo_operations.c</t>
-  </si>
-  <si>
-    <t>mesh_refresh.c</t>
-  </si>
-  <si>
-    <t>update</t>
-  </si>
-  <si>
-    <t>mesh_operations.c</t>
-  </si>
-  <si>
-    <t>mesh_dumb_fill.c</t>
-  </si>
-  <si>
-    <t>mesh_creation.c</t>
-  </si>
-  <si>
-    <t>buffer_generated;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    glGenVertexArrays(1, me-&gt;handles + 0);</t>
-  </si>
-  <si>
-    <t>if (!me-&gt;buff_generated)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    glGenBuffers(1, me-&gt;handles + 1);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    glGenBuffers(1, me-&gt;handles + 2);</t>
-  </si>
-  <si>
-    <t>vali[1];</t>
-  </si>
-  <si>
-    <t>valf[1];</t>
-  </si>
-  <si>
-    <t>(*set_groups)(t_vao_basic *vao);</t>
-  </si>
-  <si>
-    <t>4.0</t>
-  </si>
-  <si>
-    <t>4.1</t>
-  </si>
-  <si>
-    <t>if (vao-&gt;set_groups != NULL)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>vao-&gt;set_groups</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(vao);</t>
-    </r>
-  </si>
-  <si>
-    <t>(*set_tex)(t_vao_basic *vao);</t>
-  </si>
-  <si>
-    <t>if (ntex_req != vao-&gt;vbo.ntex &amp;&amp; vao-&gt;set_tex != NULL)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>vao-&gt;set_tex</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(vao);</t>
-    </r>
-  </si>
-  <si>
-    <t>receiving: (t_vao_basic *vao)</t>
-  </si>
-  <si>
-    <t>split_vbo(vao);</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">if (vao-&gt;fill == NULL || </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>vao-&gt;fill</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(me, vao))</t>
-    </r>
-  </si>
-  <si>
-    <t>textures_calculations_utility.c</t>
-  </si>
-  <si>
-    <t>textures_calculations.c</t>
-  </si>
-  <si>
-    <t>static inline split_vbo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -946,6 +954,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF008000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF008000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -976,8 +1013,52 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1005,7 +1086,51 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="45">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1297,22 +1422,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="E104" sqref="E104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3">
@@ -1412,18 +1537,18 @@
     </row>
     <row r="16" spans="2:3">
       <c r="B16" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>137</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="2:3">
       <c r="B17" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>138</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="2:3">
@@ -1431,86 +1556,78 @@
         <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3">
-      <c r="B20" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
-      <c r="B21" t="s">
+    <row r="23" spans="2:3">
+      <c r="B23" t="s">
         <v>18</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
-      <c r="B23" s="2" t="s">
+    <row r="25" spans="2:3">
+      <c r="B25" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
-      <c r="B24" t="s">
+    <row r="26" spans="2:3">
+      <c r="B26" t="s">
         <v>17</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C26" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
-      <c r="B25" t="s">
+    <row r="27" spans="2:3">
+      <c r="B27" t="s">
         <v>30</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C27" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="2:3">
-      <c r="B27" s="2" t="s">
+    <row r="29" spans="2:3">
+      <c r="B29" s="2" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3">
-      <c r="B28" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3">
-      <c r="B29" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="30" spans="2:3">
       <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C30" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3">
-      <c r="B31" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>98</v>
+      <c r="C31" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="2:3">
-      <c r="B32" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>139</v>
+      <c r="B32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1518,210 +1635,223 @@
         <v>36</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>144</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="B34" s="11" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>99</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="B35" s="11" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>110</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="B36" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="B37" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="B38" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C38" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
-      <c r="B37" t="s">
+    <row r="39" spans="1:4">
+      <c r="B39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" t="s">
         <v>42</v>
       </c>
-      <c r="C37" t="s">
+    </row>
+    <row r="40" spans="1:4">
+      <c r="B40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
-      <c r="B38" t="s">
-        <v>32</v>
-      </c>
-      <c r="C38" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="1">
-        <v>1</v>
-      </c>
-      <c r="B40" t="s">
-        <v>38</v>
-      </c>
-      <c r="C40" t="s">
-        <v>1</v>
-      </c>
-      <c r="D40" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="1">
+    <row r="43" spans="1:4">
+      <c r="A43" s="1">
         <v>2</v>
-      </c>
-      <c r="B41" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="3">
-        <v>3</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="5" t="s">
-        <v>140</v>
       </c>
       <c r="B43" t="s">
         <v>0</v>
       </c>
       <c r="C43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="3">
+        <v>3</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B45" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" t="s">
         <v>1</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D45" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B44" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="3">
-        <v>5</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="1">
-        <v>6</v>
+      <c r="A46" s="5" t="s">
+        <v>134</v>
       </c>
       <c r="B46" t="s">
         <v>3</v>
       </c>
       <c r="C46" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="3">
+        <v>5</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1">
+        <v>6</v>
+      </c>
+      <c r="B48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" t="s">
         <v>1</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D48" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
-      <c r="B48" s="7"/>
-    </row>
-    <row r="49" spans="2:2">
-      <c r="B49" s="7"/>
+    <row r="50" spans="2:2">
+      <c r="B50" s="7"/>
     </row>
     <row r="69" spans="2:4">
       <c r="B69" s="10" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="70" spans="2:4">
       <c r="C70" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" spans="2:4">
       <c r="C71" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="72" spans="2:4">
       <c r="C72" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="73" spans="2:4">
       <c r="C73" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="74" spans="2:4">
       <c r="C74" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="75" spans="2:4">
       <c r="B75" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="76" spans="2:4">
       <c r="B76" s="7"/>
       <c r="C76" t="s">
+        <v>48</v>
+      </c>
+      <c r="D76" t="s">
         <v>49</v>
-      </c>
-      <c r="D76" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="77" spans="2:4">
       <c r="B77" s="7"/>
       <c r="C77" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D77" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="78" spans="2:4">
@@ -1730,181 +1860,181 @@
     <row r="79" spans="2:4">
       <c r="B79" s="7"/>
       <c r="C79" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="80" spans="2:4">
       <c r="C80" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="81" spans="2:8">
       <c r="B81" s="7"/>
       <c r="C81" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="82" spans="2:8">
       <c r="B82" s="7"/>
       <c r="C82" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="83" spans="2:8">
       <c r="B83" s="7"/>
       <c r="C83" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="84" spans="2:8">
       <c r="C84" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F84" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G84" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="85" spans="2:8">
       <c r="C85" t="s">
-        <v>112</v>
+        <v>150</v>
       </c>
       <c r="F85" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G85" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="H85" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="86" spans="2:8">
       <c r="B86" s="7"/>
       <c r="C86" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F86" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G86" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="H86" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="87" spans="2:8">
       <c r="B87" s="7"/>
       <c r="C87" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F87" t="s">
+        <v>103</v>
+      </c>
+      <c r="G87" t="s">
+        <v>107</v>
+      </c>
+      <c r="H87" t="s">
         <v>109</v>
-      </c>
-      <c r="G87" t="s">
-        <v>114</v>
-      </c>
-      <c r="H87" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="88" spans="2:8">
       <c r="B88" s="7"/>
       <c r="C88" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F88" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G88" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="H88" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="89" spans="2:8">
       <c r="B89" s="7"/>
       <c r="C89" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="90" spans="2:8">
       <c r="B90" s="7"/>
       <c r="C90" s="8" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="91" spans="2:8">
       <c r="B91" s="7"/>
       <c r="C91" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F91" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G91" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="H91" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="92" spans="2:8">
       <c r="B92" s="7"/>
       <c r="C92" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="F92" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G92" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="H92" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="93" spans="2:8">
       <c r="B93" s="7"/>
       <c r="C93" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F93" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G93" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="H93" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="94" spans="2:8">
       <c r="B94" s="7"/>
       <c r="C94" s="8" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="95" spans="2:8">
       <c r="B95" s="7"/>
       <c r="C95" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="96" spans="2:8">
       <c r="B96" s="7"/>
       <c r="C96" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="97" spans="2:7">
       <c r="B97" s="7"/>
       <c r="C97" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="98" spans="2:7">
@@ -1915,173 +2045,173 @@
     </row>
     <row r="100" spans="2:7">
       <c r="B100" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C100" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="101" spans="2:7">
       <c r="B101" s="7"/>
       <c r="C101" t="s">
-        <v>104</v>
+        <v>149</v>
       </c>
     </row>
     <row r="102" spans="2:7">
       <c r="B102" s="7"/>
       <c r="F102" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G102" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="103" spans="2:7">
       <c r="B103" s="7"/>
       <c r="C103" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="104" spans="2:7">
       <c r="B104" s="7"/>
       <c r="C104" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="105" spans="2:7">
       <c r="B105" s="7"/>
       <c r="C105" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="106" spans="2:7">
       <c r="C106" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="107" spans="2:7">
       <c r="C107" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="108" spans="2:7">
       <c r="C108" t="s">
-        <v>102</v>
+        <v>152</v>
       </c>
     </row>
     <row r="109" spans="2:7">
       <c r="C109" t="s">
-        <v>103</v>
+        <v>151</v>
       </c>
     </row>
     <row r="112" spans="2:7">
       <c r="B112" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C112" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="113" spans="2:7">
       <c r="C113" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="114" spans="2:7">
       <c r="C114" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="115" spans="2:7">
       <c r="C115" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="116" spans="2:7">
       <c r="C116" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="117" spans="2:7">
       <c r="C117" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="118" spans="2:7">
       <c r="C118" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="119" spans="2:7">
       <c r="C119" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="120" spans="2:7">
       <c r="C120" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="121" spans="2:7">
       <c r="C121" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="122" spans="2:7">
       <c r="C122" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="123" spans="2:7">
       <c r="B123" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C123" s="9" t="s">
         <v>87</v>
-      </c>
-      <c r="C123" s="9" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="124" spans="2:7">
       <c r="C124" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="125" spans="2:7">
       <c r="C125" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="126" spans="2:7">
       <c r="C126" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="127" spans="2:7">
       <c r="C127" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="128" spans="2:7">
       <c r="C128" t="s">
-        <v>100</v>
+        <v>148</v>
       </c>
       <c r="F128" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G128" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="129" spans="2:7">
       <c r="C129" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="133" spans="2:7">
       <c r="B133" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C133" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="134" spans="2:7">
@@ -2090,16 +2220,16 @@
         <v>28</v>
       </c>
       <c r="D134" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="135" spans="2:7">
       <c r="B135" s="7"/>
       <c r="C135" t="s">
+        <v>51</v>
+      </c>
+      <c r="D135" t="s">
         <v>52</v>
-      </c>
-      <c r="D135" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="136" spans="2:7">
@@ -2108,13 +2238,13 @@
         <v>18</v>
       </c>
       <c r="D136" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F136" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G136" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="137" spans="2:7">
@@ -2123,7 +2253,7 @@
         <v>18</v>
       </c>
       <c r="D137" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="138" spans="2:7">
@@ -2132,151 +2262,166 @@
     <row r="139" spans="2:7">
       <c r="B139" s="7"/>
       <c r="C139" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="140" spans="2:7">
       <c r="B140" s="7"/>
       <c r="C140" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="141" spans="2:7">
       <c r="B141" s="7"/>
       <c r="C141" t="s">
-        <v>101</v>
+        <v>147</v>
       </c>
     </row>
     <row r="142" spans="2:7">
       <c r="B142" s="7"/>
       <c r="C142" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="143" spans="2:7">
       <c r="B143" s="7"/>
       <c r="C143" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="144" spans="2:7">
       <c r="B144" s="7"/>
       <c r="C144" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="145" spans="2:7">
       <c r="B145" s="7"/>
       <c r="C145" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="146" spans="2:7">
       <c r="B146" s="7"/>
       <c r="C146" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="147" spans="2:7">
       <c r="B147" s="7"/>
       <c r="C147" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="148" spans="2:7">
       <c r="B148" s="7"/>
       <c r="C148" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F148" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="G148" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="149" spans="2:7">
       <c r="F149" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="G149" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="150" spans="2:7">
       <c r="F150" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="G150" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="151" spans="2:7">
       <c r="F151" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="G151" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="152" spans="2:7">
       <c r="F152" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="G152" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="154" spans="2:7">
       <c r="F154" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G154" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="155" spans="2:7">
       <c r="F155" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G155" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="156" spans="2:7">
       <c r="F156" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G156" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>